<commit_message>
update ppt ujian 3
</commit_message>
<xml_diff>
--- a/Data Hasil Pengujian Evaluasi TA.xlsx
+++ b/Data Hasil Pengujian Evaluasi TA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7920" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7920" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Variable View" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>...menemukan bahwa sistem ini berguna dalam pekerjaan saya.</t>
+  </si>
+  <si>
+    <t>Sepenuhnya benar</t>
   </si>
 </sst>
 </file>
@@ -1854,6 +1857,574 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Akurasi!$F$27:$F$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Salah</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sebagian benar</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sepenuhnya benar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Akurasi!$G$27:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5AAD-483F-ADEC-72D61709D747}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="id-ID"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Akurasi!$K$27:$K$29</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Salah</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sebagian benar</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sepenuhnya benar</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Akurasi!$L$27:$L$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-19B2-4971-9D57-579FC9D0AFF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="id-ID"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2094,6 +2665,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
@@ -4690,6 +5341,1044 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5385,6 +7074,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8637,7 +10391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -10615,8 +12369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11912,29 +13666,47 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>52</v>
+      </c>
       <c r="G27">
         <f>SUM(C22:G22)</f>
         <v>2</v>
       </c>
+      <c r="K27" t="s">
+        <v>52</v>
+      </c>
       <c r="L27">
         <f>SUM(H22:L22)</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>53</v>
+      </c>
       <c r="G28">
         <f>SUM(C23:G23)</f>
         <v>88</v>
       </c>
+      <c r="K28" t="s">
+        <v>53</v>
+      </c>
       <c r="L28">
         <f>SUM(H23:L23)</f>
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>90</v>
+      </c>
       <c r="G29">
         <f>SUM(C24:G24)</f>
         <v>10</v>
+      </c>
+      <c r="K29" t="s">
+        <v>90</v>
       </c>
       <c r="L29">
         <f>SUM(H24:L24)</f>
@@ -12073,6 +13845,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>